<commit_message>
critical bugs fixed, dictionaries updated, buttons adjusted
</commit_message>
<xml_diff>
--- a/dictionary_for_database.xlsx
+++ b/dictionary_for_database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shapovv/PycharmProjects/Radost/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41902CEF-B3A8-CC4D-BB5E-87BA90CB5185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B14BE82E-A9F7-FA4E-998E-69DF37024A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="100" yWindow="500" windowWidth="17340" windowHeight="17500" xr2:uid="{5429B6A6-3AB4-3F43-B880-B81809A67136}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="145">
   <si>
     <t>analogue_1</t>
   </si>
@@ -449,9 +449,6 @@
     <t>2) Введите ваше ФИО на английском языке в формате "Ivanov_A_S"</t>
   </si>
   <si>
-    <t>&lt;b&gt;Приступим к созданию вашего технического задания.&lt;/b&gt;\n Сейчас мы поэтапно пройдём по всем пунктам, начиная с титульного листа и заканчивая списком литературы. Следуйте дальнейшим указаниям и подсказкам. \n\nВ любом месте вы можете остановиться и отправить ответ позднее, а если захотите закончить и получить не док онца заполненный документ, введите /stop. \n\nЕсли вы хотите пропустить любой шаг, необходимо отправить в ответ любой символ, тогда вы сможете заполнить этот раздел самостоятельно в итоговом документе.</t>
-  </si>
-  <si>
     <t>&lt;b&gt;Отлично! Теперь заполним титульный лист.&lt;/b&gt;\n\nВведите полное название ВУЗа, например "Национальный исследовательский университет Высшая Школа Экономики"</t>
   </si>
   <si>
@@ -480,6 +477,12 @@
   </si>
   <si>
     <t>Добро пожаловать в бота &lt;b&gt;"Радость Научника"&lt;/b&gt;!\n\nЯ помогу вам создать профессиональную техническую документацию, включая Титульный лист, Техническое задание и Пояснительную записку. Все документы будут оформлены согласно ГОСТам, что обеспечит точность и качество вашей работы.\n\nДля начала создания документации рыберите, какой документ вы бы хотели создать и следуйте дальнейшим инструкциям. Я буду задавать вам вопросы и предоставлю готовые документы на основе ваших ответов.\n\nС &lt;b&gt;"Радостью Научника"&lt;/b&gt; ваша техническая документация будет всегда на высоте!</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Напоминание:&lt;/b&gt; не забудбте заполнить до конца все приложения и проставить количество листов на листе утверждения!</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Приступим к созданию вашего технического задания.&lt;/b&gt;\nСейчас мы поэтапно пройдём по всем пунктам, начиная с титульного листа и заканчивая списком литературы. Следуйте дальнейшим указаниям и подсказкам. \n\nВ любом месте вы можете остановиться и отправить ответ позднее, а если захотите закончить и получить не док онца заполненный документ, введите /stop. \n\nЕсли вы хотите пропустить любой шаг, необходимо отправить в ответ любой символ, тогда вы сможете заполнить этот раздел самостоятельно в итоговом документе.</t>
   </si>
 </sst>
 </file>
@@ -861,10 +864,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90374932-3BD5-7B45-8650-D95A2EC64DDF}">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -884,7 +887,7 @@
     <row r="2" spans="1:4" ht="170" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -892,12 +895,12 @@
     <row r="3" spans="1:4" ht="153" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>51</v>
       </c>
@@ -913,7 +916,7 @@
         <v>('&lt;b&gt;Чтобы в дальнейшем корректно сохранить документ, ответьте на два вопроса:&lt;/b&gt;\n\n1) Введите год выполнения работы, например "2023":', 'year'),</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>130</v>
       </c>
@@ -1014,7 +1017,7 @@
         <v>48</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C11" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1654,7 +1657,7 @@
         <v>31</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C51" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1663,6 +1666,11 @@
       <c r="D51" s="1" t="str">
         <f t="shared" si="3"/>
         <v>('&lt;b&gt;Заключительный раздел "Список использованных источников".&lt;/b&gt;\n\nПо умолчанию в него включены 12 основных ГОСТ-ов, по которым оформляется пояснительная записка. Чтобы добавить свои источники, введите их через перевод строки в одном сообщении\n\nПодсказка: чтобы оформить список литературы по ГОСТу рекомендуем воспользоваться сайтом - https://open-resource.ru/spisok-literatury/:', 'sources'),</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="B52" s="1" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1887,7 +1895,7 @@
         <v>48</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C15" s="1" t="str">
         <f>"'"&amp;A15&amp;"': '',"</f>
@@ -2211,7 +2219,7 @@
         <v>43</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C6" s="1" t="str">
         <f t="shared" ref="C6:C18" si="0">"'"&amp;A6&amp;"': '',"</f>
@@ -2291,7 +2299,7 @@
         <v>48</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C11" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2384,10 +2392,10 @@
     </row>
     <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>140</v>
       </c>
       <c r="C17" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2419,7 +2427,7 @@
         <v>103</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C19" s="1" t="str">
         <f t="shared" ref="C19:C24" si="6">"'"&amp;A19&amp;"': '',"</f>
@@ -2435,7 +2443,7 @@
         <v>104</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C20" s="1" t="str">
         <f t="shared" si="6"/>
@@ -2691,7 +2699,7 @@
         <v>31</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C36" s="1" t="str">
         <f t="shared" si="8"/>
@@ -2707,7 +2715,7 @@
         <v>111</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C37" s="1" t="str">
         <f t="shared" si="8"/>

</xml_diff>